<commit_message>
Sample 01 (add header text, in progress..)
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample01-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample01-from-config-file.xlsx
@@ -460,7 +460,7 @@
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="1"/>
+    <sheetView workbookViewId="0" showGridLines="1" view="pageLayout"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -549,7 +549,9 @@
   <autoFilter ref="A1:E1"/>
   <pageMargins left="0.787400" right="0.787400" top="0.787400" bottom="0.787400" header="0.315" footer="0.315"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <headerFooter>
+    <oddHeader>&amp;CInventory</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add Minichart location by column and absolute coordenates. Modify sample 6 for demostrate how to use. Modify xsd schema and realtionated classes.
</commit_message>
<xml_diff>
--- a/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample01-from-config-file.xlsx
+++ b/source/samples/export/iTinExportEngineSamples/output/EPPlusSamples/sample01-from-config-file.xlsx
@@ -6,7 +6,6 @@
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
-    <sheet name="PivotSimple" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Inventory'!$A$1:$E$1</definedName>
@@ -14,9 +13,6 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Inventory'!$1:$1</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
-  <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
-  </pivotCaches>
 </workbook>
 </file>
 
@@ -296,166 +292,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <pivotSource xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-    <c:name>[]PivotSimple!PerEmploee</c:name>
-    <c:fmtId val="0"/>
-  </pivotSource>
-  <c:chart>
-    <pivotFmts xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-      </c:pivotFmt>
-    </pivotFmts>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <ser xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>
-              </c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'PivotSimple'!$A$1</c:f>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'PivotSimple'!$B$1</c:f>
-              <c:numCache>General</c:numCache>
-            </c:numRef>
-          </c:val>
-        </ser>
-      </c:pieChart>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <graphicFrame xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="PivotChart"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="SomeUser" refreshedDate="40504.582403125001" createdVersion="1" refreshedVersion="3" recordCount="5" upgradeOnRefresh="1">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A1:H501" sheet="Inventory"/>
-  </cacheSource>
-  <cacheFields count="8">
-    <cacheField name="ID" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Product" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Quantity" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Price" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Value" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Column6" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Column7" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Column8" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="0"/>
-</file>
-
-<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PerEmploee" cacheId="1" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Data" createdVersion="4" showMemberPropertyTips="0" useAutoFormatting="1" itemPrintTitles="1" indent="0" compact="0" compactData="0" gridDropZones="1">
-  <location ref="A1" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0" axis="axisRow">
-      <items count="1">
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0" dataField="1"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields>
-    <field x="3"/>
-  </rowFields>
-  <dataFields>
-    <dataField fld="5" numFmtId="3" name="Column6"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium9" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:E5"/>
@@ -553,16 +389,4 @@
     <oddHeader>&amp;CInventory</oddHeader>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <headerFooter/>
-  <drawing r:id="rId2"/>
-</worksheet>
 </file>
</xml_diff>